<commit_message>
add final draft #1 or paycheck breakdown chart
</commit_message>
<xml_diff>
--- a/eda-and-visualization/data/dc_paycheck_basedata.xlsx
+++ b/eda-and-visualization/data/dc_paycheck_basedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pauljeffries/Desktop/personal/personal_code/on_github/data-science-toolkit/eda-and-visualization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10F4111-F506-9244-B8BD-2658F37A32DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52AF734-73D7-D647-B71B-16722A456251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21400" windowHeight="14120" xr2:uid="{FC54C8B1-4993-EC42-AEB8-E18EC45E67FD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Gross Bi-Weekly Pay</t>
   </si>
@@ -91,6 +91,34 @@
   </si>
   <si>
     <t>Total (Pre-401k Match)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hypothetical Bi-Weekly Paycheck of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="15"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Average</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DC Resident</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -100,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +144,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,11 +230,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -201,6 +256,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -210,11 +268,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +586,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325BC79E-F4D6-DE42-8682-AE887FF077E2}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -535,188 +594,198 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E4" s="4">
         <v>256.60252881983934</v>
       </c>
-      <c r="E2" s="6">
-        <f>D2/$D$11</f>
+      <c r="F4" s="6">
+        <f>E4/$E$13</f>
         <v>8.9200000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="1" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E5" s="4">
         <v>13.51</v>
       </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E10" si="0">D3/$D$11</f>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:F12" si="0">E5/$E$13</f>
         <v>4.6963371933333329E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="1" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E6" s="4">
         <v>52.64</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>1.8298681706666667E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="1" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>3.4761933333333334E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E8" s="4">
         <v>220.07</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>7.6500586686666663E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E9" s="4">
         <v>371.38</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>0.12909886801333334</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E10" s="4">
         <v>124.56</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>4.3299464160000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E11" s="4">
         <v>1836.9474355281352</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>0.63855844290666663</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="3" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E12" s="4">
         <v>115.06839857391898</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="10" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11">
-        <f>SUM(D2:D9)</f>
+      <c r="E13" s="8">
+        <f>SUM(E4:E11)</f>
         <v>2876.7099643479746</v>
       </c>
-      <c r="E11" s="12">
-        <f>SUM(E2:E10)</f>
+      <c r="F13" s="9">
+        <f>SUM(F4:F12)</f>
         <v>1.04</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="4">
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D11" formulaRange="1"/>
+    <ignoredError sqref="E13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>